<commit_message>
novo bot no telegram
</commit_message>
<xml_diff>
--- a/Robo_PUT_PETR4.xlsx
+++ b/Robo_PUT_PETR4.xlsx
@@ -763,7 +763,7 @@
         <v>0.002</v>
       </c>
       <c r="G4">
-        <v>-0.62</v>
+        <v>-0.63</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -792,7 +792,7 @@
         <v>0.002</v>
       </c>
       <c r="G5">
-        <v>-0.61</v>
+        <v>-0.62</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -821,7 +821,7 @@
         <v>0.0029</v>
       </c>
       <c r="G6">
-        <v>-0.59</v>
+        <v>-0.6</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -914,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -989,19 +989,19 @@
         <v>90</v>
       </c>
       <c r="E12">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="F12">
-        <v>0.003</v>
+        <v>0.0022</v>
       </c>
       <c r="G12">
-        <v>-0.48</v>
+        <v>-0.49</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1024,10 +1024,10 @@
         <v>0.0036</v>
       </c>
       <c r="G13">
-        <v>-0.46</v>
+        <v>-0.47</v>
       </c>
       <c r="H13">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1053,10 +1053,10 @@
         <v>0.0034</v>
       </c>
       <c r="G14">
-        <v>-0.44</v>
+        <v>-0.45</v>
       </c>
       <c r="H14">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1082,7 +1082,7 @@
         <v>0.004</v>
       </c>
       <c r="G15">
-        <v>-0.42</v>
+        <v>-0.43</v>
       </c>
       <c r="H15">
         <v>0.03</v>
@@ -1111,10 +1111,10 @@
         <v>0.0033</v>
       </c>
       <c r="G16">
-        <v>-0.41</v>
+        <v>-0.42</v>
       </c>
       <c r="H16">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1140,10 +1140,10 @@
         <v>0.0032</v>
       </c>
       <c r="G17">
-        <v>-0.4</v>
+        <v>-0.41</v>
       </c>
       <c r="H17">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1169,10 +1169,10 @@
         <v>0.0032</v>
       </c>
       <c r="G18">
-        <v>-0.39</v>
+        <v>-0.4</v>
       </c>
       <c r="H18">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1198,13 +1198,13 @@
         <v>0.0038</v>
       </c>
       <c r="G19">
-        <v>-0.38</v>
+        <v>-0.39</v>
       </c>
       <c r="H19">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1227,10 +1227,10 @@
         <v>0.0043</v>
       </c>
       <c r="G20">
-        <v>-0.37</v>
+        <v>-0.38</v>
       </c>
       <c r="H20">
-        <v>0.19</v>
+        <v>0.15</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1256,10 +1256,10 @@
         <v>0.0042</v>
       </c>
       <c r="G21">
-        <v>-0.36</v>
+        <v>-0.37</v>
       </c>
       <c r="H21">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1285,10 +1285,10 @@
         <v>0.0042</v>
       </c>
       <c r="G22">
-        <v>-0.35</v>
+        <v>-0.36</v>
       </c>
       <c r="H22">
-        <v>0.35</v>
+        <v>0.27</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1314,10 +1314,10 @@
         <v>0.0047</v>
       </c>
       <c r="G23">
-        <v>-0.34</v>
+        <v>-0.35</v>
       </c>
       <c r="H23">
-        <v>0.46</v>
+        <v>0.36</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1343,10 +1343,10 @@
         <v>0.0058</v>
       </c>
       <c r="G24">
-        <v>-0.33</v>
+        <v>-0.34</v>
       </c>
       <c r="H24">
-        <v>0.6</v>
+        <v>0.48</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1372,10 +1372,10 @@
         <v>0.0057</v>
       </c>
       <c r="G25">
-        <v>-0.32</v>
+        <v>-0.33</v>
       </c>
       <c r="H25">
-        <v>0.77</v>
+        <v>0.62</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1404,7 +1404,7 @@
         <v>-0.31</v>
       </c>
       <c r="H26">
-        <v>1.24</v>
+        <v>1.01</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1433,7 +1433,7 @@
         <v>-0.3</v>
       </c>
       <c r="H27">
-        <v>1.55</v>
+        <v>1.27</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>-0.29</v>
       </c>
       <c r="H28">
-        <v>1.92</v>
+        <v>1.59</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1488,10 +1488,10 @@
         <v>0.008</v>
       </c>
       <c r="G29">
-        <v>-0.28</v>
+        <v>-0.29</v>
       </c>
       <c r="H29">
-        <v>2.36</v>
+        <v>1.96</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -1511,19 +1511,19 @@
         <v>90</v>
       </c>
       <c r="E30">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="F30">
-        <v>0.0074</v>
+        <v>0.0068</v>
       </c>
       <c r="G30">
-        <v>-0.27</v>
+        <v>-0.28</v>
       </c>
       <c r="H30">
-        <v>2.86</v>
+        <v>2.39</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>4100</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1540,19 +1540,19 @@
         <v>90</v>
       </c>
       <c r="E31">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="F31">
-        <v>0.0078</v>
+        <v>0.0068</v>
       </c>
       <c r="G31">
-        <v>-0.26</v>
+        <v>-0.27</v>
       </c>
       <c r="H31">
-        <v>3.45</v>
+        <v>2.9</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>34800</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1575,10 +1575,10 @@
         <v>0.0077</v>
       </c>
       <c r="G32">
-        <v>-0.25</v>
+        <v>-0.26</v>
       </c>
       <c r="H32">
-        <v>4.12</v>
+        <v>3.48</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -1598,19 +1598,19 @@
         <v>90</v>
       </c>
       <c r="E33">
-        <v>0.21</v>
+        <v>0.15</v>
       </c>
       <c r="F33">
-        <v>0.0106</v>
+        <v>0.0076</v>
       </c>
       <c r="G33">
-        <v>-0.24</v>
+        <v>-0.25</v>
       </c>
       <c r="H33">
-        <v>4.88</v>
+        <v>4.15</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1633,10 +1633,10 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="G34">
-        <v>-0.23</v>
+        <v>-0.24</v>
       </c>
       <c r="H34">
-        <v>5.74</v>
+        <v>4.9</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -1656,19 +1656,19 @@
         <v>90</v>
       </c>
       <c r="E35">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="F35">
-        <v>0.0094</v>
+        <v>0.0089</v>
       </c>
       <c r="G35">
-        <v>-0.22</v>
+        <v>-0.23</v>
       </c>
       <c r="H35">
-        <v>6.71</v>
+        <v>5.76</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1685,19 +1685,19 @@
         <v>90</v>
       </c>
       <c r="E36">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="F36">
-        <v>0.0102</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="G36">
-        <v>-0.21</v>
+        <v>-0.22</v>
       </c>
       <c r="H36">
-        <v>7.78</v>
+        <v>6.71</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1720,10 +1720,10 @@
         <v>0.0106</v>
       </c>
       <c r="G37">
-        <v>-0.2</v>
+        <v>-0.21</v>
       </c>
       <c r="H37">
-        <v>8.960000000000001</v>
+        <v>7.76</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -1743,19 +1743,19 @@
         <v>90</v>
       </c>
       <c r="E38">
-        <v>0.25</v>
+        <v>0.22</v>
       </c>
       <c r="F38">
-        <v>0.0119</v>
+        <v>0.0105</v>
       </c>
       <c r="G38">
-        <v>-0.19</v>
+        <v>-0.2</v>
       </c>
       <c r="H38">
-        <v>10.25</v>
+        <v>8.93</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1778,13 +1778,13 @@
         <v>0.0113</v>
       </c>
       <c r="G39">
-        <v>-0.18</v>
+        <v>-0.19</v>
       </c>
       <c r="H39">
-        <v>11.65</v>
+        <v>10.2</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1801,19 +1801,19 @@
         <v>90</v>
       </c>
       <c r="E40">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="F40">
-        <v>0.014</v>
+        <v>0.0126</v>
       </c>
       <c r="G40">
-        <v>-0.17</v>
+        <v>-0.18</v>
       </c>
       <c r="H40">
-        <v>13.17</v>
+        <v>11.58</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1836,10 +1836,10 @@
         <v>0.0138</v>
       </c>
       <c r="G41">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="H41">
-        <v>14.79</v>
+        <v>13.07</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -1859,19 +1859,19 @@
         <v>90</v>
       </c>
       <c r="E42">
-        <v>0.37</v>
+        <v>0.32</v>
       </c>
       <c r="F42">
-        <v>0.0168</v>
+        <v>0.0145</v>
       </c>
       <c r="G42">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="H42">
-        <v>16.53</v>
+        <v>14.67</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>68600</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1888,19 +1888,19 @@
         <v>90</v>
       </c>
       <c r="E43">
-        <v>0.39</v>
+        <v>0.34</v>
       </c>
       <c r="F43">
-        <v>0.0175</v>
+        <v>0.0153</v>
       </c>
       <c r="G43">
-        <v>-0.14</v>
+        <v>-0.15</v>
       </c>
       <c r="H43">
-        <v>18.37</v>
+        <v>16.37</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1917,19 +1917,19 @@
         <v>90</v>
       </c>
       <c r="E44">
-        <v>0.43</v>
+        <v>0.38</v>
       </c>
       <c r="F44">
-        <v>0.0191</v>
+        <v>0.0169</v>
       </c>
       <c r="G44">
-        <v>-0.13</v>
+        <v>-0.14</v>
       </c>
       <c r="H44">
-        <v>20.31</v>
+        <v>18.18</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1952,10 +1952,10 @@
         <v>0.0207</v>
       </c>
       <c r="G45">
-        <v>-0.12</v>
+        <v>-0.13</v>
       </c>
       <c r="H45">
-        <v>22.34</v>
+        <v>20.09</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -1972,22 +1972,22 @@
         <v>89</v>
       </c>
       <c r="D46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E46">
-        <v>0.52</v>
+        <v>0.46</v>
       </c>
       <c r="F46">
-        <v>0.0226</v>
+        <v>0.02</v>
       </c>
       <c r="G46">
-        <v>-0.11</v>
+        <v>-0.12</v>
       </c>
       <c r="H46">
-        <v>24.46</v>
+        <v>22.09</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>60300</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2004,19 +2004,19 @@
         <v>91</v>
       </c>
       <c r="E47">
-        <v>0.5600000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F47">
-        <v>0.0241</v>
+        <v>0.0215</v>
       </c>
       <c r="G47">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="H47">
-        <v>26.66</v>
+        <v>24.17</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2030,22 +2030,22 @@
         <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E48">
-        <v>0.62</v>
+        <v>0.57</v>
       </c>
       <c r="F48">
-        <v>0.0264</v>
+        <v>0.0243</v>
       </c>
       <c r="G48">
-        <v>-0.09</v>
+        <v>-0.1</v>
       </c>
       <c r="H48">
-        <v>28.94</v>
+        <v>26.34</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2062,19 +2062,19 @@
         <v>90</v>
       </c>
       <c r="E49">
-        <v>0.68</v>
+        <v>0.61</v>
       </c>
       <c r="F49">
-        <v>0.0286</v>
+        <v>0.0257</v>
       </c>
       <c r="G49">
-        <v>-0.08</v>
+        <v>-0.09</v>
       </c>
       <c r="H49">
-        <v>31.27</v>
+        <v>28.57</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>30100</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2091,19 +2091,19 @@
         <v>90</v>
       </c>
       <c r="E50">
-        <v>0.76</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F50">
-        <v>0.0317</v>
+        <v>0.0288</v>
       </c>
       <c r="G50">
-        <v>-0.07000000000000001</v>
+        <v>-0.09</v>
       </c>
       <c r="H50">
-        <v>33.65</v>
+        <v>30.86</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>61300</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2120,19 +2120,19 @@
         <v>90</v>
       </c>
       <c r="E51">
-        <v>0.85</v>
+        <v>0.74</v>
       </c>
       <c r="F51">
-        <v>0.0351</v>
+        <v>0.0305</v>
       </c>
       <c r="G51">
-        <v>-0.06</v>
+        <v>-0.08</v>
       </c>
       <c r="H51">
-        <v>36.08</v>
+        <v>33.21</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>400</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2149,19 +2149,19 @@
         <v>90</v>
       </c>
       <c r="E52">
-        <v>0.98</v>
+        <v>0.9</v>
       </c>
       <c r="F52">
-        <v>0.0396</v>
+        <v>0.0364</v>
       </c>
       <c r="G52">
-        <v>-0.04</v>
+        <v>-0.06</v>
       </c>
       <c r="H52">
-        <v>41.02</v>
+        <v>38.03</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>11600</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2178,19 +2178,19 @@
         <v>90</v>
       </c>
       <c r="E53">
-        <v>1.09</v>
+        <v>0.99</v>
       </c>
       <c r="F53">
-        <v>0.0436</v>
+        <v>0.0396</v>
       </c>
       <c r="G53">
-        <v>-0.04</v>
+        <v>-0.05</v>
       </c>
       <c r="H53">
-        <v>43.51</v>
+        <v>40.47</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2207,19 +2207,19 @@
         <v>90</v>
       </c>
       <c r="E54">
-        <v>1.19</v>
+        <v>1.06</v>
       </c>
       <c r="F54">
-        <v>0.0471</v>
+        <v>0.042</v>
       </c>
       <c r="G54">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="H54">
-        <v>46</v>
+        <v>42.93</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2236,19 +2236,19 @@
         <v>90</v>
       </c>
       <c r="E55">
-        <v>1.28</v>
+        <v>1.19</v>
       </c>
       <c r="F55">
-        <v>0.0502</v>
+        <v>0.0467</v>
       </c>
       <c r="G55">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="H55">
-        <v>48.48</v>
+        <v>45.39</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2268,10 +2268,10 @@
         <v>92</v>
       </c>
       <c r="G56">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="H56">
-        <v>48.48</v>
+        <v>45.39</v>
       </c>
       <c r="I56" t="s">
         <v>92</v>
@@ -2291,19 +2291,19 @@
         <v>90</v>
       </c>
       <c r="E57">
-        <v>1.43</v>
+        <v>1.3</v>
       </c>
       <c r="F57">
-        <v>0.0555</v>
+        <v>0.0505</v>
       </c>
       <c r="G57">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="H57">
-        <v>50.95</v>
+        <v>47.85</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2320,19 +2320,19 @@
         <v>90</v>
       </c>
       <c r="E58">
-        <v>1.55</v>
+        <v>1.38</v>
       </c>
       <c r="F58">
-        <v>0.0596</v>
+        <v>0.0531</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="H58">
-        <v>53.38</v>
+        <v>50.29</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>42100</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2349,19 +2349,19 @@
         <v>90</v>
       </c>
       <c r="E59">
-        <v>1.66</v>
+        <v>1.53</v>
       </c>
       <c r="F59">
-        <v>0.06320000000000001</v>
+        <v>0.0583</v>
       </c>
       <c r="G59">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H59">
-        <v>55.79</v>
+        <v>52.7</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2378,19 +2378,19 @@
         <v>90</v>
       </c>
       <c r="E60">
-        <v>1.81</v>
+        <v>1.65</v>
       </c>
       <c r="F60">
-        <v>0.0683</v>
+        <v>0.0623</v>
       </c>
       <c r="G60">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="H60">
-        <v>58.14</v>
+        <v>55.09</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2407,19 +2407,19 @@
         <v>90</v>
       </c>
       <c r="E61">
-        <v>1.95</v>
+        <v>1.79</v>
       </c>
       <c r="F61">
-        <v>0.07290000000000001</v>
+        <v>0.0669</v>
       </c>
       <c r="G61">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="H61">
-        <v>60.45</v>
+        <v>57.43</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>13000</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2436,19 +2436,19 @@
         <v>90</v>
       </c>
       <c r="E62">
-        <v>2.1</v>
+        <v>1.91</v>
       </c>
       <c r="F62">
-        <v>0.07779999999999999</v>
+        <v>0.0707</v>
       </c>
       <c r="G62">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="H62">
-        <v>62.7</v>
+        <v>59.72</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>6200</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2465,19 +2465,19 @@
         <v>90</v>
       </c>
       <c r="E63">
-        <v>2.47</v>
+        <v>2.25</v>
       </c>
       <c r="F63">
-        <v>0.0898</v>
+        <v>0.0818</v>
       </c>
       <c r="G63">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="H63">
-        <v>67.01000000000001</v>
+        <v>64.15000000000001</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>500</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2497,10 +2497,10 @@
         <v>92</v>
       </c>
       <c r="G64">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="H64">
-        <v>67.01000000000001</v>
+        <v>64.15000000000001</v>
       </c>
       <c r="I64" t="s">
         <v>92</v>
@@ -2526,10 +2526,10 @@
         <v>0.0951</v>
       </c>
       <c r="G65">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="H65">
-        <v>69.06</v>
+        <v>66.27</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -2549,19 +2549,19 @@
         <v>90</v>
       </c>
       <c r="E66">
-        <v>2.79</v>
+        <v>2.53</v>
       </c>
       <c r="F66">
-        <v>0.09959999999999999</v>
+        <v>0.09039999999999999</v>
       </c>
       <c r="G66">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H66">
-        <v>71.03</v>
+        <v>68.31999999999999</v>
       </c>
       <c r="I66">
-        <v>0</v>
+        <v>64200</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2584,10 +2584,10 @@
         <v>0.1123</v>
       </c>
       <c r="G67">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H67">
-        <v>74.73999999999999</v>
+        <v>72.19</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -2610,10 +2610,10 @@
         <v>92</v>
       </c>
       <c r="G68">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H68">
-        <v>74.73999999999999</v>
+        <v>72.19</v>
       </c>
       <c r="I68" t="s">
         <v>92</v>
@@ -2639,10 +2639,10 @@
         <v>0.105</v>
       </c>
       <c r="G69">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="H69">
-        <v>76.48</v>
+        <v>74.02</v>
       </c>
       <c r="I69">
         <v>0</v>
@@ -2668,10 +2668,10 @@
         <v>0.1169</v>
       </c>
       <c r="G70">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="H70">
-        <v>78.13</v>
+        <v>75.77</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -2697,10 +2697,10 @@
         <v>0.1332</v>
       </c>
       <c r="G71">
-        <v>0.14</v>
+        <v>0.12</v>
       </c>
       <c r="H71">
-        <v>81.19</v>
+        <v>79.02</v>
       </c>
       <c r="I71">
         <v>0</v>
@@ -2726,10 +2726,10 @@
         <v>0.1383</v>
       </c>
       <c r="G72">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="H72">
-        <v>83.92</v>
+        <v>81.95</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -2755,10 +2755,10 @@
         <v>0.1416</v>
       </c>
       <c r="G73">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="H73">
-        <v>86.34</v>
+        <v>84.56999999999999</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -2781,10 +2781,10 @@
         <v>92</v>
       </c>
       <c r="G74">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="H74">
-        <v>86.34</v>
+        <v>84.56999999999999</v>
       </c>
       <c r="I74" t="s">
         <v>92</v>
@@ -2810,10 +2810,10 @@
         <v>0.1379</v>
       </c>
       <c r="G75">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="H75">
-        <v>87.44</v>
+        <v>85.77</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -2839,10 +2839,10 @@
         <v>0.171</v>
       </c>
       <c r="G76">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="H76">
-        <v>88.47</v>
+        <v>86.89</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -2868,10 +2868,10 @@
         <v>0.2686</v>
       </c>
       <c r="G77">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="H77">
-        <v>90.31999999999999</v>
+        <v>88.92</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -2897,10 +2897,10 @@
         <v>0.2835</v>
       </c>
       <c r="G78">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="H78">
-        <v>91.15000000000001</v>
+        <v>89.84</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -2926,10 +2926,10 @@
         <v>0.5562</v>
       </c>
       <c r="G79">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="H79">
-        <v>91.92</v>
+        <v>90.69</v>
       </c>
       <c r="I79">
         <v>0</v>
@@ -2952,10 +2952,10 @@
         <v>92</v>
       </c>
       <c r="G80">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="H80">
-        <v>93.29000000000001</v>
+        <v>92.22</v>
       </c>
       <c r="I80" t="s">
         <v>92</v>
@@ -2981,10 +2981,10 @@
         <v>0</v>
       </c>
       <c r="G81">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="H81">
-        <v>94.45999999999999</v>
+        <v>93.54000000000001</v>
       </c>
       <c r="I81">
         <v>0</v>

</xml_diff>

<commit_message>
Atualizacao diaria do sistema
</commit_message>
<xml_diff>
--- a/Robo_PUT_PETR4.xlsx
+++ b/Robo_PUT_PETR4.xlsx
@@ -705,7 +705,7 @@
         <v>0.0021</v>
       </c>
       <c r="G2">
-        <v>-0.64</v>
+        <v>-0.65</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -734,7 +734,7 @@
         <v>0.0021</v>
       </c>
       <c r="G3">
-        <v>-0.63</v>
+        <v>-0.64</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -786,10 +786,10 @@
         <v>90</v>
       </c>
       <c r="E5">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F5">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G5">
         <v>-0.62</v>
@@ -821,7 +821,7 @@
         <v>0.0029</v>
       </c>
       <c r="G6">
-        <v>-0.6</v>
+        <v>-0.61</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -850,7 +850,7 @@
         <v>0.0018</v>
       </c>
       <c r="G7">
-        <v>-0.58</v>
+        <v>-0.59</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -879,7 +879,7 @@
         <v>0.0017</v>
       </c>
       <c r="G8">
-        <v>-0.5600000000000001</v>
+        <v>-0.57</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -908,13 +908,13 @@
         <v>0.0017</v>
       </c>
       <c r="G9">
-        <v>-0.54</v>
+        <v>-0.55</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -937,7 +937,7 @@
         <v>0.0048</v>
       </c>
       <c r="G10">
-        <v>-0.52</v>
+        <v>-0.53</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -966,7 +966,7 @@
         <v>0.0031</v>
       </c>
       <c r="G11">
-        <v>-0.5</v>
+        <v>-0.51</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1001,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>10000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1018,10 +1018,10 @@
         <v>90</v>
       </c>
       <c r="E13">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F13">
-        <v>0.0036</v>
+        <v>0.0021</v>
       </c>
       <c r="G13">
         <v>-0.47</v>
@@ -1053,7 +1053,7 @@
         <v>0.0034</v>
       </c>
       <c r="G14">
-        <v>-0.45</v>
+        <v>-0.46</v>
       </c>
       <c r="H14">
         <v>0.01</v>
@@ -1076,16 +1076,16 @@
         <v>90</v>
       </c>
       <c r="E15">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="F15">
-        <v>0.004</v>
+        <v>0.0027</v>
       </c>
       <c r="G15">
-        <v>-0.43</v>
+        <v>-0.44</v>
       </c>
       <c r="H15">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1111,10 +1111,10 @@
         <v>0.0033</v>
       </c>
       <c r="G16">
-        <v>-0.42</v>
+        <v>-0.43</v>
       </c>
       <c r="H16">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1140,10 +1140,10 @@
         <v>0.0032</v>
       </c>
       <c r="G17">
-        <v>-0.41</v>
+        <v>-0.42</v>
       </c>
       <c r="H17">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1169,10 +1169,10 @@
         <v>0.0032</v>
       </c>
       <c r="G18">
-        <v>-0.4</v>
+        <v>-0.41</v>
       </c>
       <c r="H18">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1192,19 +1192,19 @@
         <v>90</v>
       </c>
       <c r="E19">
+        <v>0.05</v>
+      </c>
+      <c r="F19">
+        <v>0.0031</v>
+      </c>
+      <c r="G19">
+        <v>-0.4</v>
+      </c>
+      <c r="H19">
         <v>0.06</v>
       </c>
-      <c r="F19">
-        <v>0.0038</v>
-      </c>
-      <c r="G19">
-        <v>-0.39</v>
-      </c>
-      <c r="H19">
-        <v>0.11</v>
-      </c>
       <c r="I19">
-        <v>7000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1227,10 +1227,10 @@
         <v>0.0043</v>
       </c>
       <c r="G20">
-        <v>-0.38</v>
+        <v>-0.39</v>
       </c>
       <c r="H20">
-        <v>0.15</v>
+        <v>0.09</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1250,16 +1250,16 @@
         <v>90</v>
       </c>
       <c r="E21">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="F21">
-        <v>0.0042</v>
+        <v>0.0036</v>
       </c>
       <c r="G21">
-        <v>-0.37</v>
+        <v>-0.38</v>
       </c>
       <c r="H21">
-        <v>0.2</v>
+        <v>0.12</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1285,10 +1285,10 @@
         <v>0.0042</v>
       </c>
       <c r="G22">
-        <v>-0.36</v>
+        <v>-0.37</v>
       </c>
       <c r="H22">
-        <v>0.27</v>
+        <v>0.17</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1308,16 +1308,16 @@
         <v>90</v>
       </c>
       <c r="E23">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="F23">
-        <v>0.0047</v>
+        <v>0.0035</v>
       </c>
       <c r="G23">
-        <v>-0.35</v>
+        <v>-0.36</v>
       </c>
       <c r="H23">
-        <v>0.36</v>
+        <v>0.23</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1337,16 +1337,16 @@
         <v>90</v>
       </c>
       <c r="E24">
-        <v>0.1</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F24">
-        <v>0.0058</v>
+        <v>0.0041</v>
       </c>
       <c r="G24">
-        <v>-0.34</v>
+        <v>-0.35</v>
       </c>
       <c r="H24">
-        <v>0.48</v>
+        <v>0.3</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1366,16 +1366,16 @@
         <v>90</v>
       </c>
       <c r="E25">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F25">
-        <v>0.0057</v>
+        <v>0.0046</v>
       </c>
       <c r="G25">
-        <v>-0.33</v>
+        <v>-0.34</v>
       </c>
       <c r="H25">
-        <v>0.62</v>
+        <v>0.4</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -1395,16 +1395,16 @@
         <v>90</v>
       </c>
       <c r="E26">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="F26">
-        <v>0.005</v>
+        <v>0.0044</v>
       </c>
       <c r="G26">
-        <v>-0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="H26">
-        <v>1.01</v>
+        <v>0.68</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1424,16 +1424,16 @@
         <v>90</v>
       </c>
       <c r="E27">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="F27">
-        <v>0.006</v>
+        <v>0.0049</v>
       </c>
       <c r="G27">
-        <v>-0.3</v>
+        <v>-0.31</v>
       </c>
       <c r="H27">
-        <v>1.27</v>
+        <v>0.87</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1453,16 +1453,16 @@
         <v>90</v>
       </c>
       <c r="E28">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="F28">
-        <v>0.0059</v>
+        <v>0.0049</v>
       </c>
       <c r="G28">
-        <v>-0.29</v>
+        <v>-0.31</v>
       </c>
       <c r="H28">
-        <v>1.59</v>
+        <v>1.09</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1488,10 +1488,10 @@
         <v>0.008</v>
       </c>
       <c r="G29">
-        <v>-0.29</v>
+        <v>-0.3</v>
       </c>
       <c r="H29">
-        <v>1.96</v>
+        <v>1.37</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -1511,19 +1511,19 @@
         <v>90</v>
       </c>
       <c r="E30">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F30">
-        <v>0.0068</v>
+        <v>0.0063</v>
       </c>
       <c r="G30">
-        <v>-0.28</v>
+        <v>-0.29</v>
       </c>
       <c r="H30">
-        <v>2.39</v>
+        <v>1.7</v>
       </c>
       <c r="I30">
-        <v>4100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1546,13 +1546,13 @@
         <v>0.0068</v>
       </c>
       <c r="G31">
-        <v>-0.27</v>
+        <v>-0.28</v>
       </c>
       <c r="H31">
-        <v>2.9</v>
+        <v>2.09</v>
       </c>
       <c r="I31">
-        <v>34800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1569,16 +1569,16 @@
         <v>90</v>
       </c>
       <c r="E32">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="F32">
-        <v>0.0077</v>
+        <v>0.0067</v>
       </c>
       <c r="G32">
-        <v>-0.26</v>
+        <v>-0.27</v>
       </c>
       <c r="H32">
-        <v>3.48</v>
+        <v>2.54</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -1598,19 +1598,19 @@
         <v>90</v>
       </c>
       <c r="E33">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="F33">
-        <v>0.0076</v>
+        <v>0.0066</v>
       </c>
       <c r="G33">
-        <v>-0.25</v>
+        <v>-0.26</v>
       </c>
       <c r="H33">
-        <v>4.15</v>
+        <v>3.07</v>
       </c>
       <c r="I33">
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1627,16 +1627,16 @@
         <v>90</v>
       </c>
       <c r="E34">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="F34">
-        <v>0.008999999999999999</v>
+        <v>0.008</v>
       </c>
       <c r="G34">
-        <v>-0.24</v>
+        <v>-0.25</v>
       </c>
       <c r="H34">
-        <v>4.9</v>
+        <v>3.68</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -1656,19 +1656,19 @@
         <v>90</v>
       </c>
       <c r="E35">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="F35">
-        <v>0.0089</v>
+        <v>0.008399999999999999</v>
       </c>
       <c r="G35">
-        <v>-0.23</v>
+        <v>-0.24</v>
       </c>
       <c r="H35">
-        <v>5.76</v>
+        <v>4.37</v>
       </c>
       <c r="I35">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1685,19 +1685,19 @@
         <v>90</v>
       </c>
       <c r="E36">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="F36">
-        <v>0.009299999999999999</v>
+        <v>0.0083</v>
       </c>
       <c r="G36">
-        <v>-0.22</v>
+        <v>-0.23</v>
       </c>
       <c r="H36">
-        <v>6.71</v>
+        <v>5.16</v>
       </c>
       <c r="I36">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1714,16 +1714,16 @@
         <v>90</v>
       </c>
       <c r="E37">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="F37">
-        <v>0.0106</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="G37">
-        <v>-0.21</v>
+        <v>-0.22</v>
       </c>
       <c r="H37">
-        <v>7.76</v>
+        <v>6.04</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -1743,19 +1743,19 @@
         <v>90</v>
       </c>
       <c r="E38">
-        <v>0.22</v>
+        <v>0.21</v>
       </c>
       <c r="F38">
-        <v>0.0105</v>
+        <v>0.01</v>
       </c>
       <c r="G38">
-        <v>-0.2</v>
+        <v>-0.21</v>
       </c>
       <c r="H38">
-        <v>8.93</v>
+        <v>7.02</v>
       </c>
       <c r="I38">
-        <v>4200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1772,19 +1772,19 @@
         <v>90</v>
       </c>
       <c r="E39">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="F39">
-        <v>0.0113</v>
+        <v>0.0094</v>
       </c>
       <c r="G39">
-        <v>-0.19</v>
+        <v>-0.2</v>
       </c>
       <c r="H39">
-        <v>10.2</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="I39">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1801,19 +1801,19 @@
         <v>90</v>
       </c>
       <c r="E40">
-        <v>0.27</v>
+        <v>0.25</v>
       </c>
       <c r="F40">
-        <v>0.0126</v>
+        <v>0.0116</v>
       </c>
       <c r="G40">
-        <v>-0.18</v>
+        <v>-0.19</v>
       </c>
       <c r="H40">
-        <v>11.58</v>
+        <v>9.31</v>
       </c>
       <c r="I40">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1830,16 +1830,16 @@
         <v>90</v>
       </c>
       <c r="E41">
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="F41">
-        <v>0.0138</v>
+        <v>0.011</v>
       </c>
       <c r="G41">
-        <v>-0.17</v>
+        <v>-0.18</v>
       </c>
       <c r="H41">
-        <v>13.07</v>
+        <v>10.61</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -1859,19 +1859,19 @@
         <v>90</v>
       </c>
       <c r="E42">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
       <c r="F42">
-        <v>0.0145</v>
+        <v>0.0136</v>
       </c>
       <c r="G42">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="H42">
-        <v>14.67</v>
+        <v>12.02</v>
       </c>
       <c r="I42">
-        <v>68600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1888,19 +1888,19 @@
         <v>90</v>
       </c>
       <c r="E43">
-        <v>0.34</v>
+        <v>0.3</v>
       </c>
       <c r="F43">
-        <v>0.0153</v>
+        <v>0.0135</v>
       </c>
       <c r="G43">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="H43">
-        <v>16.37</v>
+        <v>13.55</v>
       </c>
       <c r="I43">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1917,19 +1917,19 @@
         <v>90</v>
       </c>
       <c r="E44">
-        <v>0.38</v>
+        <v>0.35</v>
       </c>
       <c r="F44">
-        <v>0.0169</v>
+        <v>0.0156</v>
       </c>
       <c r="G44">
-        <v>-0.14</v>
+        <v>-0.16</v>
       </c>
       <c r="H44">
-        <v>18.18</v>
+        <v>15.18</v>
       </c>
       <c r="I44">
-        <v>3500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1943,19 +1943,19 @@
         <v>89</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E45">
-        <v>0.47</v>
+        <v>0.39</v>
       </c>
       <c r="F45">
-        <v>0.0207</v>
+        <v>0.0171</v>
       </c>
       <c r="G45">
-        <v>-0.13</v>
+        <v>-0.15</v>
       </c>
       <c r="H45">
-        <v>20.09</v>
+        <v>16.92</v>
       </c>
       <c r="I45">
         <v>0</v>
@@ -1981,13 +1981,13 @@
         <v>0.02</v>
       </c>
       <c r="G46">
-        <v>-0.12</v>
+        <v>-0.14</v>
       </c>
       <c r="H46">
-        <v>22.09</v>
+        <v>18.76</v>
       </c>
       <c r="I46">
-        <v>60300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2001,22 +2001,22 @@
         <v>89</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E47">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
       <c r="F47">
-        <v>0.0215</v>
+        <v>0.0185</v>
       </c>
       <c r="G47">
-        <v>-0.11</v>
+        <v>-0.13</v>
       </c>
       <c r="H47">
-        <v>24.17</v>
+        <v>20.69</v>
       </c>
       <c r="I47">
-        <v>1100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2033,19 +2033,19 @@
         <v>91</v>
       </c>
       <c r="E48">
-        <v>0.57</v>
+        <v>0.51</v>
       </c>
       <c r="F48">
-        <v>0.0243</v>
+        <v>0.0217</v>
       </c>
       <c r="G48">
-        <v>-0.1</v>
+        <v>-0.12</v>
       </c>
       <c r="H48">
-        <v>26.34</v>
+        <v>22.72</v>
       </c>
       <c r="I48">
-        <v>1500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2059,22 +2059,22 @@
         <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E49">
-        <v>0.61</v>
+        <v>0.5</v>
       </c>
       <c r="F49">
-        <v>0.0257</v>
+        <v>0.0211</v>
       </c>
       <c r="G49">
-        <v>-0.09</v>
+        <v>-0.11</v>
       </c>
       <c r="H49">
-        <v>28.57</v>
+        <v>24.83</v>
       </c>
       <c r="I49">
-        <v>30100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2091,19 +2091,19 @@
         <v>90</v>
       </c>
       <c r="E50">
-        <v>0.6899999999999999</v>
+        <v>0.61</v>
       </c>
       <c r="F50">
-        <v>0.0288</v>
+        <v>0.0254</v>
       </c>
       <c r="G50">
-        <v>-0.09</v>
+        <v>-0.1</v>
       </c>
       <c r="H50">
-        <v>30.86</v>
+        <v>27.02</v>
       </c>
       <c r="I50">
-        <v>61300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2120,19 +2120,19 @@
         <v>90</v>
       </c>
       <c r="E51">
-        <v>0.74</v>
+        <v>0.65</v>
       </c>
       <c r="F51">
-        <v>0.0305</v>
+        <v>0.0268</v>
       </c>
       <c r="G51">
-        <v>-0.08</v>
+        <v>-0.09</v>
       </c>
       <c r="H51">
-        <v>33.21</v>
+        <v>29.28</v>
       </c>
       <c r="I51">
-        <v>400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2149,19 +2149,19 @@
         <v>90</v>
       </c>
       <c r="E52">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="F52">
-        <v>0.0364</v>
+        <v>0.0323</v>
       </c>
       <c r="G52">
-        <v>-0.06</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="H52">
-        <v>38.03</v>
+        <v>33.96</v>
       </c>
       <c r="I52">
-        <v>11600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2178,19 +2178,19 @@
         <v>90</v>
       </c>
       <c r="E53">
-        <v>0.99</v>
+        <v>0.86</v>
       </c>
       <c r="F53">
-        <v>0.0396</v>
+        <v>0.0344</v>
       </c>
       <c r="G53">
-        <v>-0.05</v>
+        <v>-0.06</v>
       </c>
       <c r="H53">
-        <v>40.47</v>
+        <v>36.37</v>
       </c>
       <c r="I53">
-        <v>9000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2207,19 +2207,19 @@
         <v>90</v>
       </c>
       <c r="E54">
-        <v>1.06</v>
+        <v>0.96</v>
       </c>
       <c r="F54">
-        <v>0.042</v>
+        <v>0.038</v>
       </c>
       <c r="G54">
-        <v>-0.04</v>
+        <v>-0.05</v>
       </c>
       <c r="H54">
-        <v>42.93</v>
+        <v>38.81</v>
       </c>
       <c r="I54">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2236,19 +2236,19 @@
         <v>90</v>
       </c>
       <c r="E55">
-        <v>1.19</v>
+        <v>1.06</v>
       </c>
       <c r="F55">
-        <v>0.0467</v>
+        <v>0.0416</v>
       </c>
       <c r="G55">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="H55">
-        <v>45.39</v>
+        <v>41.26</v>
       </c>
       <c r="I55">
-        <v>3600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2268,10 +2268,10 @@
         <v>92</v>
       </c>
       <c r="G56">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="H56">
-        <v>45.39</v>
+        <v>41.26</v>
       </c>
       <c r="I56" t="s">
         <v>92</v>
@@ -2291,19 +2291,19 @@
         <v>90</v>
       </c>
       <c r="E57">
-        <v>1.3</v>
+        <v>1.15</v>
       </c>
       <c r="F57">
-        <v>0.0505</v>
+        <v>0.0447</v>
       </c>
       <c r="G57">
-        <v>-0.02</v>
+        <v>-0.03</v>
       </c>
       <c r="H57">
-        <v>47.85</v>
+        <v>43.73</v>
       </c>
       <c r="I57">
-        <v>1100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2320,19 +2320,19 @@
         <v>90</v>
       </c>
       <c r="E58">
-        <v>1.38</v>
+        <v>1.23</v>
       </c>
       <c r="F58">
-        <v>0.0531</v>
+        <v>0.0473</v>
       </c>
       <c r="G58">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="H58">
-        <v>50.29</v>
+        <v>46.2</v>
       </c>
       <c r="I58">
-        <v>42100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2349,19 +2349,19 @@
         <v>90</v>
       </c>
       <c r="E59">
-        <v>1.53</v>
+        <v>1.37</v>
       </c>
       <c r="F59">
-        <v>0.0583</v>
+        <v>0.0522</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>-0.01</v>
       </c>
       <c r="H59">
-        <v>52.7</v>
+        <v>48.66</v>
       </c>
       <c r="I59">
-        <v>2500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2378,19 +2378,19 @@
         <v>90</v>
       </c>
       <c r="E60">
-        <v>1.65</v>
+        <v>1.48</v>
       </c>
       <c r="F60">
-        <v>0.0623</v>
+        <v>0.0558</v>
       </c>
       <c r="G60">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="H60">
-        <v>55.09</v>
+        <v>51.1</v>
       </c>
       <c r="I60">
-        <v>8700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2407,19 +2407,19 @@
         <v>90</v>
       </c>
       <c r="E61">
-        <v>1.79</v>
+        <v>1.57</v>
       </c>
       <c r="F61">
-        <v>0.0669</v>
+        <v>0.0587</v>
       </c>
       <c r="G61">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H61">
-        <v>57.43</v>
+        <v>53.51</v>
       </c>
       <c r="I61">
-        <v>13000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2436,19 +2436,19 @@
         <v>90</v>
       </c>
       <c r="E62">
-        <v>1.91</v>
+        <v>1.75</v>
       </c>
       <c r="F62">
-        <v>0.0707</v>
+        <v>0.0648</v>
       </c>
       <c r="G62">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="H62">
-        <v>59.72</v>
+        <v>55.89</v>
       </c>
       <c r="I62">
-        <v>6200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2465,19 +2465,19 @@
         <v>90</v>
       </c>
       <c r="E63">
-        <v>2.25</v>
+        <v>2</v>
       </c>
       <c r="F63">
-        <v>0.0818</v>
+        <v>0.0727</v>
       </c>
       <c r="G63">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="H63">
-        <v>64.15000000000001</v>
+        <v>60.51</v>
       </c>
       <c r="I63">
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2497,10 +2497,10 @@
         <v>92</v>
       </c>
       <c r="G64">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="H64">
-        <v>64.15000000000001</v>
+        <v>60.51</v>
       </c>
       <c r="I64" t="s">
         <v>92</v>
@@ -2520,16 +2520,16 @@
         <v>90</v>
       </c>
       <c r="E65">
-        <v>2.64</v>
+        <v>2.17</v>
       </c>
       <c r="F65">
-        <v>0.0951</v>
+        <v>0.07820000000000001</v>
       </c>
       <c r="G65">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="H65">
-        <v>66.27</v>
+        <v>62.74</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -2549,19 +2549,19 @@
         <v>90</v>
       </c>
       <c r="E66">
-        <v>2.53</v>
+        <v>2.34</v>
       </c>
       <c r="F66">
-        <v>0.09039999999999999</v>
+        <v>0.08359999999999999</v>
       </c>
       <c r="G66">
-        <v>0.07000000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="H66">
-        <v>68.31999999999999</v>
+        <v>64.91</v>
       </c>
       <c r="I66">
-        <v>64200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2578,16 +2578,16 @@
         <v>90</v>
       </c>
       <c r="E67">
-        <v>3.2</v>
+        <v>2.58</v>
       </c>
       <c r="F67">
-        <v>0.1123</v>
+        <v>0.0905</v>
       </c>
       <c r="G67">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H67">
-        <v>72.19</v>
+        <v>69.05</v>
       </c>
       <c r="I67">
         <v>0</v>
@@ -2610,10 +2610,10 @@
         <v>92</v>
       </c>
       <c r="G68">
-        <v>0.09</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H68">
-        <v>72.19</v>
+        <v>69.05</v>
       </c>
       <c r="I68" t="s">
         <v>92</v>
@@ -2633,16 +2633,16 @@
         <v>90</v>
       </c>
       <c r="E69">
-        <v>3.02</v>
+        <v>2.65</v>
       </c>
       <c r="F69">
-        <v>0.105</v>
+        <v>0.0922</v>
       </c>
       <c r="G69">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H69">
-        <v>74.02</v>
+        <v>71.01000000000001</v>
       </c>
       <c r="I69">
         <v>0</v>
@@ -2662,16 +2662,16 @@
         <v>90</v>
       </c>
       <c r="E70">
-        <v>3.39</v>
+        <v>2.9</v>
       </c>
       <c r="F70">
-        <v>0.1169</v>
+        <v>0.1</v>
       </c>
       <c r="G70">
-        <v>0.11</v>
+        <v>0.09</v>
       </c>
       <c r="H70">
-        <v>75.77</v>
+        <v>72.89</v>
       </c>
       <c r="I70">
         <v>0</v>
@@ -2691,16 +2691,16 @@
         <v>90</v>
       </c>
       <c r="E71">
-        <v>3.93</v>
+        <v>3.28</v>
       </c>
       <c r="F71">
-        <v>0.1332</v>
+        <v>0.1112</v>
       </c>
       <c r="G71">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="H71">
-        <v>79.02</v>
+        <v>76.42</v>
       </c>
       <c r="I71">
         <v>0</v>
@@ -2720,16 +2720,16 @@
         <v>90</v>
       </c>
       <c r="E72">
-        <v>4.15</v>
+        <v>3.86</v>
       </c>
       <c r="F72">
-        <v>0.1383</v>
+        <v>0.1287</v>
       </c>
       <c r="G72">
-        <v>0.14</v>
+        <v>0.13</v>
       </c>
       <c r="H72">
-        <v>81.95</v>
+        <v>79.63</v>
       </c>
       <c r="I72">
         <v>0</v>
@@ -2749,16 +2749,16 @@
         <v>90</v>
       </c>
       <c r="E73">
-        <v>4.32</v>
+        <v>4.03</v>
       </c>
       <c r="F73">
-        <v>0.1416</v>
+        <v>0.1321</v>
       </c>
       <c r="G73">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="H73">
-        <v>84.56999999999999</v>
+        <v>82.51000000000001</v>
       </c>
       <c r="I73">
         <v>0</v>
@@ -2781,10 +2781,10 @@
         <v>92</v>
       </c>
       <c r="G74">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="H74">
-        <v>84.56999999999999</v>
+        <v>82.51000000000001</v>
       </c>
       <c r="I74" t="s">
         <v>92</v>
@@ -2810,10 +2810,10 @@
         <v>0.1379</v>
       </c>
       <c r="G75">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="H75">
-        <v>85.77</v>
+        <v>83.83</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -2839,10 +2839,10 @@
         <v>0.171</v>
       </c>
       <c r="G76">
-        <v>0.18</v>
+        <v>0.16</v>
       </c>
       <c r="H76">
-        <v>86.89</v>
+        <v>85.08</v>
       </c>
       <c r="I76">
         <v>0</v>
@@ -2868,10 +2868,10 @@
         <v>0.2686</v>
       </c>
       <c r="G77">
-        <v>0.2</v>
+        <v>0.18</v>
       </c>
       <c r="H77">
-        <v>88.92</v>
+        <v>87.34999999999999</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -2897,10 +2897,10 @@
         <v>0.2835</v>
       </c>
       <c r="G78">
-        <v>0.21</v>
+        <v>0.19</v>
       </c>
       <c r="H78">
-        <v>89.84</v>
+        <v>88.38</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -2920,16 +2920,16 @@
         <v>90</v>
       </c>
       <c r="E79">
-        <v>17.8</v>
+        <v>5.45</v>
       </c>
       <c r="F79">
-        <v>0.5562</v>
+        <v>0.1703</v>
       </c>
       <c r="G79">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="H79">
-        <v>90.69</v>
+        <v>89.34</v>
       </c>
       <c r="I79">
         <v>0</v>
@@ -2952,10 +2952,10 @@
         <v>92</v>
       </c>
       <c r="G80">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="H80">
-        <v>92.22</v>
+        <v>91.06999999999999</v>
       </c>
       <c r="I80" t="s">
         <v>92</v>
@@ -2981,10 +2981,10 @@
         <v>0</v>
       </c>
       <c r="G81">
-        <v>0.26</v>
+        <v>0.24</v>
       </c>
       <c r="H81">
-        <v>93.54000000000001</v>
+        <v>92.56</v>
       </c>
       <c r="I81">
         <v>0</v>

</xml_diff>

<commit_message>
Atulizacao nas paginas posicaoBBAS e criacao mapaitub4
</commit_message>
<xml_diff>
--- a/Robo_PUT_PETR4.xlsx
+++ b/Robo_PUT_PETR4.xlsx
@@ -705,7 +705,7 @@
         <v>0.0021</v>
       </c>
       <c r="G2">
-        <v>-0.65</v>
+        <v>-0.66</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -734,7 +734,7 @@
         <v>0.0021</v>
       </c>
       <c r="G3">
-        <v>-0.64</v>
+        <v>-0.65</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>0.002</v>
       </c>
       <c r="G4">
-        <v>-0.63</v>
+        <v>-0.64</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -792,13 +792,13 @@
         <v>0.001</v>
       </c>
       <c r="G5">
-        <v>-0.62</v>
+        <v>-0.63</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -821,7 +821,7 @@
         <v>0.0029</v>
       </c>
       <c r="G6">
-        <v>-0.61</v>
+        <v>-0.62</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -844,19 +844,19 @@
         <v>90</v>
       </c>
       <c r="E7">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F7">
-        <v>0.0018</v>
+        <v>0.0009</v>
       </c>
       <c r="G7">
-        <v>-0.59</v>
+        <v>-0.6</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -879,13 +879,13 @@
         <v>0.0017</v>
       </c>
       <c r="G8">
-        <v>-0.57</v>
+        <v>-0.58</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -908,13 +908,13 @@
         <v>0.0017</v>
       </c>
       <c r="G9">
-        <v>-0.55</v>
+        <v>-0.5600000000000001</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>10200</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -931,19 +931,19 @@
         <v>90</v>
       </c>
       <c r="E10">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="F10">
-        <v>0.0048</v>
+        <v>0.0016</v>
       </c>
       <c r="G10">
-        <v>-0.53</v>
+        <v>-0.54</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -960,19 +960,19 @@
         <v>90</v>
       </c>
       <c r="E11">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="F11">
-        <v>0.0031</v>
+        <v>0.0015</v>
       </c>
       <c r="G11">
-        <v>-0.51</v>
+        <v>-0.53</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>176000</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -989,19 +989,19 @@
         <v>90</v>
       </c>
       <c r="E12">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="F12">
-        <v>0.0022</v>
+        <v>0.003</v>
       </c>
       <c r="G12">
-        <v>-0.49</v>
+        <v>-0.51</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1024,13 +1024,13 @@
         <v>0.0021</v>
       </c>
       <c r="G13">
-        <v>-0.47</v>
+        <v>-0.49</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>3800</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1047,19 +1047,19 @@
         <v>90</v>
       </c>
       <c r="E14">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="F14">
-        <v>0.0034</v>
+        <v>0.0028</v>
       </c>
       <c r="G14">
-        <v>-0.46</v>
+        <v>-0.47</v>
       </c>
       <c r="H14">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1082,13 +1082,13 @@
         <v>0.0027</v>
       </c>
       <c r="G15">
-        <v>-0.44</v>
+        <v>-0.45</v>
       </c>
       <c r="H15">
         <v>0.01</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>900</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1111,10 +1111,10 @@
         <v>0.0033</v>
       </c>
       <c r="G16">
-        <v>-0.43</v>
+        <v>-0.44</v>
       </c>
       <c r="H16">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1140,10 +1140,10 @@
         <v>0.0032</v>
       </c>
       <c r="G17">
-        <v>-0.42</v>
+        <v>-0.43</v>
       </c>
       <c r="H17">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1169,10 +1169,10 @@
         <v>0.0032</v>
       </c>
       <c r="G18">
-        <v>-0.41</v>
+        <v>-0.42</v>
       </c>
       <c r="H18">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1198,13 +1198,13 @@
         <v>0.0031</v>
       </c>
       <c r="G19">
-        <v>-0.4</v>
+        <v>-0.42</v>
       </c>
       <c r="H19">
-        <v>0.06</v>
+        <v>0.03</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1227,10 +1227,10 @@
         <v>0.0043</v>
       </c>
       <c r="G20">
-        <v>-0.39</v>
+        <v>-0.41</v>
       </c>
       <c r="H20">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1256,10 +1256,10 @@
         <v>0.0036</v>
       </c>
       <c r="G21">
-        <v>-0.38</v>
+        <v>-0.4</v>
       </c>
       <c r="H21">
-        <v>0.12</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1285,10 +1285,10 @@
         <v>0.0042</v>
       </c>
       <c r="G22">
-        <v>-0.37</v>
+        <v>-0.39</v>
       </c>
       <c r="H22">
-        <v>0.17</v>
+        <v>0.09</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1314,13 +1314,13 @@
         <v>0.0035</v>
       </c>
       <c r="G23">
-        <v>-0.36</v>
+        <v>-0.38</v>
       </c>
       <c r="H23">
-        <v>0.23</v>
+        <v>0.13</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>700</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1343,10 +1343,10 @@
         <v>0.0041</v>
       </c>
       <c r="G24">
-        <v>-0.35</v>
+        <v>-0.37</v>
       </c>
       <c r="H24">
-        <v>0.3</v>
+        <v>0.17</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1366,19 +1366,19 @@
         <v>90</v>
       </c>
       <c r="E25">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F25">
-        <v>0.0046</v>
+        <v>0.004</v>
       </c>
       <c r="G25">
-        <v>-0.34</v>
+        <v>-0.36</v>
       </c>
       <c r="H25">
-        <v>0.4</v>
+        <v>0.23</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>122000</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1401,13 +1401,13 @@
         <v>0.0044</v>
       </c>
       <c r="G26">
-        <v>-0.32</v>
+        <v>-0.34</v>
       </c>
       <c r="H26">
-        <v>0.68</v>
+        <v>0.41</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>23300</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1430,13 +1430,13 @@
         <v>0.0049</v>
       </c>
       <c r="G27">
-        <v>-0.31</v>
+        <v>-0.33</v>
       </c>
       <c r="H27">
-        <v>0.87</v>
+        <v>0.53</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1459,10 +1459,10 @@
         <v>0.0049</v>
       </c>
       <c r="G28">
-        <v>-0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="H28">
-        <v>1.09</v>
+        <v>0.68</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1482,19 +1482,19 @@
         <v>90</v>
       </c>
       <c r="E29">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="F29">
-        <v>0.008</v>
+        <v>0.0053</v>
       </c>
       <c r="G29">
-        <v>-0.3</v>
+        <v>-0.32</v>
       </c>
       <c r="H29">
-        <v>1.37</v>
+        <v>0.86</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1511,19 +1511,19 @@
         <v>90</v>
       </c>
       <c r="E30">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="F30">
-        <v>0.0063</v>
+        <v>0.0053</v>
       </c>
       <c r="G30">
-        <v>-0.29</v>
+        <v>-0.31</v>
       </c>
       <c r="H30">
-        <v>1.7</v>
+        <v>1.08</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>25200</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1540,19 +1540,19 @@
         <v>90</v>
       </c>
       <c r="E31">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
       <c r="F31">
-        <v>0.0068</v>
+        <v>0.0057</v>
       </c>
       <c r="G31">
-        <v>-0.28</v>
+        <v>-0.3</v>
       </c>
       <c r="H31">
-        <v>2.09</v>
+        <v>1.35</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>29000</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1569,19 +1569,19 @@
         <v>90</v>
       </c>
       <c r="E32">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F32">
-        <v>0.0067</v>
+        <v>0.0062</v>
       </c>
       <c r="G32">
-        <v>-0.27</v>
+        <v>-0.29</v>
       </c>
       <c r="H32">
-        <v>2.54</v>
+        <v>1.66</v>
       </c>
       <c r="I32">
-        <v>0</v>
+        <v>214300</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1598,19 +1598,19 @@
         <v>90</v>
       </c>
       <c r="E33">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="F33">
-        <v>0.0066</v>
+        <v>0.0061</v>
       </c>
       <c r="G33">
-        <v>-0.26</v>
+        <v>-0.28</v>
       </c>
       <c r="H33">
-        <v>3.07</v>
+        <v>2.03</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>40400</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1627,19 +1627,19 @@
         <v>90</v>
       </c>
       <c r="E34">
-        <v>0.16</v>
+        <v>0.14</v>
       </c>
       <c r="F34">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
       <c r="G34">
-        <v>-0.25</v>
+        <v>-0.27</v>
       </c>
       <c r="H34">
-        <v>3.68</v>
+        <v>2.47</v>
       </c>
       <c r="I34">
-        <v>0</v>
+        <v>88600</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1656,19 +1656,19 @@
         <v>90</v>
       </c>
       <c r="E35">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="F35">
-        <v>0.008399999999999999</v>
+        <v>0.0074</v>
       </c>
       <c r="G35">
-        <v>-0.24</v>
+        <v>-0.26</v>
       </c>
       <c r="H35">
-        <v>4.37</v>
+        <v>2.97</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>18100</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1685,19 +1685,19 @@
         <v>90</v>
       </c>
       <c r="E36">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F36">
-        <v>0.0083</v>
+        <v>0.0078</v>
       </c>
       <c r="G36">
-        <v>-0.23</v>
+        <v>-0.25</v>
       </c>
       <c r="H36">
-        <v>5.16</v>
+        <v>3.54</v>
       </c>
       <c r="I36">
-        <v>0</v>
+        <v>10300</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1720,13 +1720,13 @@
         <v>0.008200000000000001</v>
       </c>
       <c r="G37">
-        <v>-0.22</v>
+        <v>-0.24</v>
       </c>
       <c r="H37">
-        <v>6.04</v>
+        <v>4.2</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1743,19 +1743,19 @@
         <v>90</v>
       </c>
       <c r="E38">
-        <v>0.21</v>
+        <v>0.18</v>
       </c>
       <c r="F38">
-        <v>0.01</v>
+        <v>0.0086</v>
       </c>
       <c r="G38">
-        <v>-0.21</v>
+        <v>-0.23</v>
       </c>
       <c r="H38">
-        <v>7.02</v>
+        <v>4.94</v>
       </c>
       <c r="I38">
-        <v>0</v>
+        <v>54500</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1772,19 +1772,19 @@
         <v>90</v>
       </c>
       <c r="E39">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="F39">
-        <v>0.0094</v>
+        <v>0.0089</v>
       </c>
       <c r="G39">
-        <v>-0.2</v>
+        <v>-0.22</v>
       </c>
       <c r="H39">
-        <v>8.109999999999999</v>
+        <v>5.77</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>9900</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1801,19 +1801,19 @@
         <v>90</v>
       </c>
       <c r="E40">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="F40">
-        <v>0.0116</v>
+        <v>0.0098</v>
       </c>
       <c r="G40">
-        <v>-0.19</v>
+        <v>-0.21</v>
       </c>
       <c r="H40">
-        <v>9.31</v>
+        <v>6.69</v>
       </c>
       <c r="I40">
-        <v>0</v>
+        <v>92200</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1830,19 +1830,19 @@
         <v>90</v>
       </c>
       <c r="E41">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="F41">
-        <v>0.011</v>
+        <v>0.0106</v>
       </c>
       <c r="G41">
-        <v>-0.18</v>
+        <v>-0.21</v>
       </c>
       <c r="H41">
-        <v>10.61</v>
+        <v>7.72</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>36900</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1859,19 +1859,19 @@
         <v>90</v>
       </c>
       <c r="E42">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="F42">
-        <v>0.0136</v>
+        <v>0.0114</v>
       </c>
       <c r="G42">
-        <v>-0.17</v>
+        <v>-0.2</v>
       </c>
       <c r="H42">
-        <v>12.02</v>
+        <v>8.84</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>111600</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1888,19 +1888,19 @@
         <v>90</v>
       </c>
       <c r="E43">
-        <v>0.3</v>
+        <v>0.26</v>
       </c>
       <c r="F43">
-        <v>0.0135</v>
+        <v>0.0117</v>
       </c>
       <c r="G43">
-        <v>-0.16</v>
+        <v>-0.19</v>
       </c>
       <c r="H43">
-        <v>13.55</v>
+        <v>10.07</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>420900</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1917,19 +1917,19 @@
         <v>90</v>
       </c>
       <c r="E44">
-        <v>0.35</v>
+        <v>0.29</v>
       </c>
       <c r="F44">
-        <v>0.0156</v>
+        <v>0.0129</v>
       </c>
       <c r="G44">
-        <v>-0.16</v>
+        <v>-0.18</v>
       </c>
       <c r="H44">
-        <v>15.18</v>
+        <v>11.4</v>
       </c>
       <c r="I44">
-        <v>0</v>
+        <v>113000</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1946,19 +1946,19 @@
         <v>90</v>
       </c>
       <c r="E45">
-        <v>0.39</v>
+        <v>0.31</v>
       </c>
       <c r="F45">
-        <v>0.0171</v>
+        <v>0.0136</v>
       </c>
       <c r="G45">
-        <v>-0.15</v>
+        <v>-0.17</v>
       </c>
       <c r="H45">
-        <v>16.92</v>
+        <v>12.83</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>26800</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1975,19 +1975,19 @@
         <v>90</v>
       </c>
       <c r="E46">
-        <v>0.46</v>
+        <v>0.35</v>
       </c>
       <c r="F46">
-        <v>0.02</v>
+        <v>0.0152</v>
       </c>
       <c r="G46">
-        <v>-0.14</v>
+        <v>-0.16</v>
       </c>
       <c r="H46">
-        <v>18.76</v>
+        <v>14.37</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>107000</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2004,19 +2004,19 @@
         <v>90</v>
       </c>
       <c r="E47">
-        <v>0.43</v>
+        <v>0.37</v>
       </c>
       <c r="F47">
-        <v>0.0185</v>
+        <v>0.0159</v>
       </c>
       <c r="G47">
-        <v>-0.13</v>
+        <v>-0.15</v>
       </c>
       <c r="H47">
-        <v>20.69</v>
+        <v>16.01</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>93900</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2030,22 +2030,22 @@
         <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E48">
-        <v>0.51</v>
+        <v>0.4</v>
       </c>
       <c r="F48">
-        <v>0.0217</v>
+        <v>0.017</v>
       </c>
       <c r="G48">
-        <v>-0.12</v>
+        <v>-0.14</v>
       </c>
       <c r="H48">
-        <v>22.72</v>
+        <v>17.75</v>
       </c>
       <c r="I48">
-        <v>0</v>
+        <v>74000</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2059,22 +2059,22 @@
         <v>89</v>
       </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E49">
-        <v>0.5</v>
+        <v>0.44</v>
       </c>
       <c r="F49">
-        <v>0.0211</v>
+        <v>0.0185</v>
       </c>
       <c r="G49">
-        <v>-0.11</v>
+        <v>-0.13</v>
       </c>
       <c r="H49">
-        <v>24.83</v>
+        <v>19.58</v>
       </c>
       <c r="I49">
-        <v>0</v>
+        <v>96700</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2091,19 +2091,19 @@
         <v>90</v>
       </c>
       <c r="E50">
-        <v>0.61</v>
+        <v>0.48</v>
       </c>
       <c r="F50">
-        <v>0.0254</v>
+        <v>0.02</v>
       </c>
       <c r="G50">
-        <v>-0.1</v>
+        <v>-0.12</v>
       </c>
       <c r="H50">
-        <v>27.02</v>
+        <v>21.51</v>
       </c>
       <c r="I50">
-        <v>0</v>
+        <v>226100</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2117,22 +2117,22 @@
         <v>89</v>
       </c>
       <c r="D51" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E51">
-        <v>0.65</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F51">
-        <v>0.0268</v>
+        <v>0.0231</v>
       </c>
       <c r="G51">
-        <v>-0.09</v>
+        <v>-0.11</v>
       </c>
       <c r="H51">
-        <v>29.28</v>
+        <v>23.51</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>15600</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2149,19 +2149,19 @@
         <v>90</v>
       </c>
       <c r="E52">
-        <v>0.8</v>
+        <v>0.64</v>
       </c>
       <c r="F52">
-        <v>0.0323</v>
+        <v>0.0259</v>
       </c>
       <c r="G52">
-        <v>-0.07000000000000001</v>
+        <v>-0.1</v>
       </c>
       <c r="H52">
-        <v>33.96</v>
+        <v>27.75</v>
       </c>
       <c r="I52">
-        <v>0</v>
+        <v>92600</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2178,19 +2178,19 @@
         <v>90</v>
       </c>
       <c r="E53">
-        <v>0.86</v>
+        <v>0.71</v>
       </c>
       <c r="F53">
-        <v>0.0344</v>
+        <v>0.0284</v>
       </c>
       <c r="G53">
-        <v>-0.06</v>
+        <v>-0.09</v>
       </c>
       <c r="H53">
-        <v>36.37</v>
+        <v>29.96</v>
       </c>
       <c r="I53">
-        <v>0</v>
+        <v>166100</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2207,19 +2207,19 @@
         <v>90</v>
       </c>
       <c r="E54">
-        <v>0.96</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F54">
-        <v>0.038</v>
+        <v>0.0321</v>
       </c>
       <c r="G54">
-        <v>-0.05</v>
+        <v>-0.08</v>
       </c>
       <c r="H54">
-        <v>38.81</v>
+        <v>32.23</v>
       </c>
       <c r="I54">
-        <v>0</v>
+        <v>83300</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2236,19 +2236,19 @@
         <v>90</v>
       </c>
       <c r="E55">
-        <v>1.06</v>
+        <v>0.83</v>
       </c>
       <c r="F55">
-        <v>0.0416</v>
+        <v>0.0325</v>
       </c>
       <c r="G55">
-        <v>-0.04</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="H55">
-        <v>41.26</v>
+        <v>34.54</v>
       </c>
       <c r="I55">
-        <v>0</v>
+        <v>161300</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2268,10 +2268,10 @@
         <v>92</v>
       </c>
       <c r="G56">
-        <v>-0.04</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="H56">
-        <v>41.26</v>
+        <v>34.54</v>
       </c>
       <c r="I56" t="s">
         <v>92</v>
@@ -2291,19 +2291,19 @@
         <v>90</v>
       </c>
       <c r="E57">
-        <v>1.15</v>
+        <v>0.92</v>
       </c>
       <c r="F57">
-        <v>0.0447</v>
+        <v>0.0357</v>
       </c>
       <c r="G57">
-        <v>-0.03</v>
+        <v>-0.06</v>
       </c>
       <c r="H57">
-        <v>43.73</v>
+        <v>36.89</v>
       </c>
       <c r="I57">
-        <v>0</v>
+        <v>140800</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2319,20 +2319,17 @@
       <c r="D58" t="s">
         <v>90</v>
       </c>
-      <c r="E58">
-        <v>1.23</v>
-      </c>
       <c r="F58">
-        <v>0.0473</v>
+        <v>0.0385</v>
       </c>
       <c r="G58">
-        <v>-0.02</v>
+        <v>-0.05</v>
       </c>
       <c r="H58">
-        <v>46.2</v>
+        <v>39.27</v>
       </c>
       <c r="I58">
-        <v>0</v>
+        <v>1035100</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2349,19 +2346,19 @@
         <v>90</v>
       </c>
       <c r="E59">
-        <v>1.37</v>
+        <v>1.08</v>
       </c>
       <c r="F59">
-        <v>0.0522</v>
+        <v>0.0411</v>
       </c>
       <c r="G59">
-        <v>-0.01</v>
+        <v>-0.04</v>
       </c>
       <c r="H59">
-        <v>48.66</v>
+        <v>41.66</v>
       </c>
       <c r="I59">
-        <v>0</v>
+        <v>41600</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2378,19 +2375,19 @@
         <v>90</v>
       </c>
       <c r="E60">
-        <v>1.48</v>
+        <v>1.2</v>
       </c>
       <c r="F60">
-        <v>0.0558</v>
+        <v>0.0453</v>
       </c>
       <c r="G60">
-        <v>-0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="H60">
-        <v>51.1</v>
+        <v>44.06</v>
       </c>
       <c r="I60">
-        <v>0</v>
+        <v>77100</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2407,19 +2404,19 @@
         <v>90</v>
       </c>
       <c r="E61">
-        <v>1.57</v>
+        <v>1.32</v>
       </c>
       <c r="F61">
-        <v>0.0587</v>
+        <v>0.0493</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>-0.02</v>
       </c>
       <c r="H61">
-        <v>53.51</v>
+        <v>46.47</v>
       </c>
       <c r="I61">
-        <v>0</v>
+        <v>161100</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2436,19 +2433,19 @@
         <v>90</v>
       </c>
       <c r="E62">
-        <v>1.75</v>
+        <v>1.4</v>
       </c>
       <c r="F62">
-        <v>0.0648</v>
+        <v>0.0519</v>
       </c>
       <c r="G62">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="H62">
-        <v>55.89</v>
+        <v>48.86</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>328400</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2465,19 +2462,19 @@
         <v>90</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>1.64</v>
       </c>
       <c r="F63">
-        <v>0.0727</v>
+        <v>0.0596</v>
       </c>
       <c r="G63">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H63">
-        <v>60.51</v>
+        <v>53.58</v>
       </c>
       <c r="I63">
-        <v>0</v>
+        <v>213200</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2497,10 +2494,10 @@
         <v>92</v>
       </c>
       <c r="G64">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H64">
-        <v>60.51</v>
+        <v>53.58</v>
       </c>
       <c r="I64" t="s">
         <v>92</v>
@@ -2520,19 +2517,19 @@
         <v>90</v>
       </c>
       <c r="E65">
-        <v>2.17</v>
+        <v>1.79</v>
       </c>
       <c r="F65">
-        <v>0.07820000000000001</v>
+        <v>0.0645</v>
       </c>
       <c r="G65">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="H65">
-        <v>62.74</v>
+        <v>55.89</v>
       </c>
       <c r="I65">
-        <v>0</v>
+        <v>128900</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2549,19 +2546,19 @@
         <v>90</v>
       </c>
       <c r="E66">
-        <v>2.34</v>
+        <v>1.92</v>
       </c>
       <c r="F66">
-        <v>0.08359999999999999</v>
+        <v>0.06859999999999999</v>
       </c>
       <c r="G66">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="H66">
-        <v>64.91</v>
+        <v>58.16</v>
       </c>
       <c r="I66">
-        <v>0</v>
+        <v>357600</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2578,19 +2575,19 @@
         <v>90</v>
       </c>
       <c r="E67">
-        <v>2.58</v>
+        <v>2.21</v>
       </c>
       <c r="F67">
-        <v>0.0905</v>
+        <v>0.0775</v>
       </c>
       <c r="G67">
-        <v>0.07000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="H67">
-        <v>69.05</v>
+        <v>62.56</v>
       </c>
       <c r="I67">
-        <v>0</v>
+        <v>61100</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2610,10 +2607,10 @@
         <v>92</v>
       </c>
       <c r="G68">
-        <v>0.07000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="H68">
-        <v>69.05</v>
+        <v>62.56</v>
       </c>
       <c r="I68" t="s">
         <v>92</v>
@@ -2633,19 +2630,19 @@
         <v>90</v>
       </c>
       <c r="E69">
-        <v>2.65</v>
+        <v>2.4</v>
       </c>
       <c r="F69">
-        <v>0.0922</v>
+        <v>0.0835</v>
       </c>
       <c r="G69">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="H69">
-        <v>71.01000000000001</v>
+        <v>64.68000000000001</v>
       </c>
       <c r="I69">
-        <v>0</v>
+        <v>20100</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2662,19 +2659,19 @@
         <v>90</v>
       </c>
       <c r="E70">
-        <v>2.9</v>
+        <v>2.56</v>
       </c>
       <c r="F70">
-        <v>0.1</v>
+        <v>0.0883</v>
       </c>
       <c r="G70">
-        <v>0.09</v>
+        <v>0.06</v>
       </c>
       <c r="H70">
-        <v>72.89</v>
+        <v>66.73</v>
       </c>
       <c r="I70">
-        <v>0</v>
+        <v>319900</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2691,19 +2688,19 @@
         <v>90</v>
       </c>
       <c r="E71">
-        <v>3.28</v>
+        <v>3.07</v>
       </c>
       <c r="F71">
-        <v>0.1112</v>
+        <v>0.1041</v>
       </c>
       <c r="G71">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
       <c r="H71">
-        <v>76.42</v>
+        <v>70.64</v>
       </c>
       <c r="I71">
-        <v>0</v>
+        <v>66100</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2720,19 +2717,19 @@
         <v>90</v>
       </c>
       <c r="E72">
-        <v>3.86</v>
+        <v>3.28</v>
       </c>
       <c r="F72">
-        <v>0.1287</v>
+        <v>0.1093</v>
       </c>
       <c r="G72">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="H72">
-        <v>79.63</v>
+        <v>74.26000000000001</v>
       </c>
       <c r="I72">
-        <v>0</v>
+        <v>60800</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2749,19 +2746,19 @@
         <v>90</v>
       </c>
       <c r="E73">
-        <v>4.03</v>
+        <v>3.66</v>
       </c>
       <c r="F73">
-        <v>0.1321</v>
+        <v>0.12</v>
       </c>
       <c r="G73">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="H73">
-        <v>82.51000000000001</v>
+        <v>77.58</v>
       </c>
       <c r="I73">
-        <v>0</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2781,10 +2778,10 @@
         <v>92</v>
       </c>
       <c r="G74">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="H74">
-        <v>82.51000000000001</v>
+        <v>77.58</v>
       </c>
       <c r="I74" t="s">
         <v>92</v>
@@ -2810,10 +2807,10 @@
         <v>0.1379</v>
       </c>
       <c r="G75">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="H75">
-        <v>83.83</v>
+        <v>79.13</v>
       </c>
       <c r="I75">
         <v>0</v>
@@ -2833,19 +2830,19 @@
         <v>90</v>
       </c>
       <c r="E76">
-        <v>5.3</v>
+        <v>4.05</v>
       </c>
       <c r="F76">
-        <v>0.171</v>
+        <v>0.1306</v>
       </c>
       <c r="G76">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="H76">
-        <v>85.08</v>
+        <v>80.59999999999999</v>
       </c>
       <c r="I76">
-        <v>0</v>
+        <v>3300</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2868,10 +2865,10 @@
         <v>0.2686</v>
       </c>
       <c r="G77">
-        <v>0.18</v>
+        <v>0.15</v>
       </c>
       <c r="H77">
-        <v>87.34999999999999</v>
+        <v>83.31</v>
       </c>
       <c r="I77">
         <v>0</v>
@@ -2891,19 +2888,19 @@
         <v>90</v>
       </c>
       <c r="E78">
-        <v>9</v>
+        <v>4.68</v>
       </c>
       <c r="F78">
-        <v>0.2835</v>
+        <v>0.1474</v>
       </c>
       <c r="G78">
-        <v>0.19</v>
+        <v>0.16</v>
       </c>
       <c r="H78">
-        <v>88.38</v>
+        <v>84.55</v>
       </c>
       <c r="I78">
-        <v>0</v>
+        <v>112300</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2920,19 +2917,19 @@
         <v>90</v>
       </c>
       <c r="E79">
-        <v>5.45</v>
+        <v>5</v>
       </c>
       <c r="F79">
-        <v>0.1703</v>
+        <v>0.1562</v>
       </c>
       <c r="G79">
-        <v>0.2</v>
+        <v>0.17</v>
       </c>
       <c r="H79">
-        <v>89.34</v>
+        <v>85.72</v>
       </c>
       <c r="I79">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -2952,10 +2949,10 @@
         <v>92</v>
       </c>
       <c r="G80">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="H80">
-        <v>91.06999999999999</v>
+        <v>87.86</v>
       </c>
       <c r="I80" t="s">
         <v>92</v>
@@ -2975,19 +2972,19 @@
         <v>90</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>5.85</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>0.1773</v>
       </c>
       <c r="G81">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="H81">
-        <v>92.56</v>
+        <v>89.73999999999999</v>
       </c>
       <c r="I81">
-        <v>0</v>
+        <v>34000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Novo grafico de rentabildiade beta
</commit_message>
<xml_diff>
--- a/Robo_PUT_PETR4.xlsx
+++ b/Robo_PUT_PETR4.xlsx
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>5000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -731,13 +731,13 @@
         <v>0.001</v>
       </c>
       <c r="G3">
-        <v>-0.65</v>
+        <v>-0.66</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>5000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -766,7 +766,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -847,13 +847,13 @@
         <v>0.0009</v>
       </c>
       <c r="G7">
-        <v>-0.6</v>
+        <v>-0.61</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>280000</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -882,7 +882,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <v>200000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>2000</v>
+        <v>81200</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -928,10 +928,10 @@
         <v>90</v>
       </c>
       <c r="E10">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F10">
-        <v>0.0016</v>
+        <v>0.0008</v>
       </c>
       <c r="G10">
         <v>-0.55</v>
@@ -940,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -969,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>600</v>
+        <v>123200</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -992,13 +992,13 @@
         <v>0.0015</v>
       </c>
       <c r="G12">
-        <v>-0.51</v>
+        <v>-0.52</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12">
-        <v>38700</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1015,10 +1015,10 @@
         <v>90</v>
       </c>
       <c r="E13">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="F13">
-        <v>0.0014</v>
+        <v>0.0007</v>
       </c>
       <c r="G13">
         <v>-0.5</v>
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>10500</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1056,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <v>2000</v>
+        <v>11100</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>143300</v>
+        <v>330900</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -1102,10 +1102,10 @@
         <v>90</v>
       </c>
       <c r="E16">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="F16">
-        <v>0.002</v>
+        <v>0.0013</v>
       </c>
       <c r="G16">
         <v>-0.45</v>
@@ -1114,7 +1114,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>125100</v>
+        <v>26400</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1131,10 +1131,10 @@
         <v>90</v>
       </c>
       <c r="E17">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="F17">
-        <v>0.0019</v>
+        <v>0.0013</v>
       </c>
       <c r="G17">
         <v>-0.44</v>
@@ -1143,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>3600</v>
+        <v>111400</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1160,10 +1160,10 @@
         <v>90</v>
       </c>
       <c r="E18">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="F18">
-        <v>0.0019</v>
+        <v>0.0013</v>
       </c>
       <c r="G18">
         <v>-0.43</v>
@@ -1172,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <v>1800</v>
+        <v>34800</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1189,19 +1189,19 @@
         <v>90</v>
       </c>
       <c r="E19">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="F19">
-        <v>0.0019</v>
+        <v>0.0012</v>
       </c>
       <c r="G19">
-        <v>-0.42</v>
+        <v>-0.43</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19">
-        <v>3700</v>
+        <v>21400</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1227,10 +1227,10 @@
         <v>-0.42</v>
       </c>
       <c r="H20">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="I20">
-        <v>60000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1259,7 +1259,7 @@
         <v>0.01</v>
       </c>
       <c r="I21">
-        <v>1000</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1285,10 +1285,10 @@
         <v>-0.4</v>
       </c>
       <c r="H22">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="I22">
-        <v>3000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1317,7 +1317,7 @@
         <v>0.02</v>
       </c>
       <c r="I23">
-        <v>29200</v>
+        <v>14900</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1343,10 +1343,10 @@
         <v>-0.38</v>
       </c>
       <c r="H24">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="I24">
-        <v>2600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1363,16 +1363,16 @@
         <v>90</v>
       </c>
       <c r="E25">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="F25">
-        <v>0.0017</v>
+        <v>0.0029</v>
       </c>
       <c r="G25">
         <v>-0.37</v>
       </c>
       <c r="H25">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="I25">
         <v>100</v>
@@ -1401,10 +1401,10 @@
         <v>-0.35</v>
       </c>
       <c r="H26">
-        <v>0.11</v>
+        <v>0.08</v>
       </c>
       <c r="I26">
-        <v>25300</v>
+        <v>73400</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1430,10 +1430,10 @@
         <v>-0.34</v>
       </c>
       <c r="H27">
-        <v>0.15</v>
+        <v>0.11</v>
       </c>
       <c r="I27">
-        <v>700</v>
+        <v>25600</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -1450,16 +1450,16 @@
         <v>90</v>
       </c>
       <c r="E28">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="F28">
-        <v>0.0016</v>
+        <v>0.0022</v>
       </c>
       <c r="G28">
         <v>-0.34</v>
       </c>
       <c r="H28">
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="I28">
         <v>1400</v>
@@ -1479,19 +1479,19 @@
         <v>90</v>
       </c>
       <c r="E29">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F29">
-        <v>0.0027</v>
+        <v>0.0016</v>
       </c>
       <c r="G29">
         <v>-0.33</v>
       </c>
       <c r="H29">
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="I29">
-        <v>5000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -1508,19 +1508,19 @@
         <v>90</v>
       </c>
       <c r="E30">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="F30">
-        <v>0.0032</v>
+        <v>0.0026</v>
       </c>
       <c r="G30">
         <v>-0.32</v>
       </c>
       <c r="H30">
-        <v>0.36</v>
+        <v>0.29</v>
       </c>
       <c r="I30">
-        <v>66400</v>
+        <v>62600</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -1546,10 +1546,10 @@
         <v>-0.31</v>
       </c>
       <c r="H31">
-        <v>0.48</v>
+        <v>0.39</v>
       </c>
       <c r="I31">
-        <v>40300</v>
+        <v>500</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -1566,19 +1566,19 @@
         <v>90</v>
       </c>
       <c r="E32">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="F32">
-        <v>0.0036</v>
+        <v>0.0031</v>
       </c>
       <c r="G32">
         <v>-0.3</v>
       </c>
       <c r="H32">
-        <v>0.63</v>
+        <v>0.51</v>
       </c>
       <c r="I32">
-        <v>2000</v>
+        <v>7000</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1604,10 +1604,10 @@
         <v>-0.29</v>
       </c>
       <c r="H33">
-        <v>0.8100000000000001</v>
+        <v>0.67</v>
       </c>
       <c r="I33">
-        <v>1600</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1624,19 +1624,19 @@
         <v>90</v>
       </c>
       <c r="E34">
-        <v>0.07000000000000001</v>
+        <v>0.06</v>
       </c>
       <c r="F34">
-        <v>0.0035</v>
+        <v>0.003</v>
       </c>
       <c r="G34">
         <v>-0.28</v>
       </c>
       <c r="H34">
-        <v>1.03</v>
+        <v>0.86</v>
       </c>
       <c r="I34">
-        <v>113700</v>
+        <v>443900</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1653,19 +1653,19 @@
         <v>90</v>
       </c>
       <c r="E35">
-        <v>0.08</v>
+        <v>0.06</v>
       </c>
       <c r="F35">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="G35">
         <v>-0.27</v>
       </c>
       <c r="H35">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="I35">
-        <v>6600</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1691,10 +1691,10 @@
         <v>-0.26</v>
       </c>
       <c r="H36">
-        <v>1.63</v>
+        <v>1.39</v>
       </c>
       <c r="I36">
-        <v>10000</v>
+        <v>136300</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1711,19 +1711,19 @@
         <v>90</v>
       </c>
       <c r="E37">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="F37">
-        <v>0.0043</v>
+        <v>0.0039</v>
       </c>
       <c r="G37">
         <v>-0.25</v>
       </c>
       <c r="H37">
-        <v>2.02</v>
+        <v>1.74</v>
       </c>
       <c r="I37">
-        <v>9600</v>
+        <v>10200</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1749,10 +1749,10 @@
         <v>-0.25</v>
       </c>
       <c r="H38">
-        <v>2.48</v>
+        <v>2.15</v>
       </c>
       <c r="I38">
-        <v>242500</v>
+        <v>290500</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1769,19 +1769,19 @@
         <v>90</v>
       </c>
       <c r="E39">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F39">
-        <v>0.0047</v>
+        <v>0.0038</v>
       </c>
       <c r="G39">
         <v>-0.24</v>
       </c>
       <c r="H39">
-        <v>3.01</v>
+        <v>2.64</v>
       </c>
       <c r="I39">
-        <v>44800</v>
+        <v>15000</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1798,19 +1798,19 @@
         <v>90</v>
       </c>
       <c r="E40">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F40">
-        <v>0.0047</v>
+        <v>0.0037</v>
       </c>
       <c r="G40">
         <v>-0.23</v>
       </c>
       <c r="H40">
-        <v>3.63</v>
+        <v>3.21</v>
       </c>
       <c r="I40">
-        <v>159900</v>
+        <v>47000</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1827,19 +1827,19 @@
         <v>90</v>
       </c>
       <c r="E41">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="F41">
-        <v>0.0055</v>
+        <v>0.0046</v>
       </c>
       <c r="G41">
         <v>-0.22</v>
       </c>
       <c r="H41">
-        <v>4.34</v>
+        <v>3.88</v>
       </c>
       <c r="I41">
-        <v>41600</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1856,19 +1856,19 @@
         <v>90</v>
       </c>
       <c r="E42">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="F42">
-        <v>0.0055</v>
+        <v>0.005</v>
       </c>
       <c r="G42">
         <v>-0.21</v>
       </c>
       <c r="H42">
-        <v>5.15</v>
+        <v>4.64</v>
       </c>
       <c r="I42">
-        <v>858100</v>
+        <v>360900</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1885,19 +1885,19 @@
         <v>90</v>
       </c>
       <c r="E43">
-        <v>0.14</v>
+        <v>0.11</v>
       </c>
       <c r="F43">
-        <v>0.0063</v>
+        <v>0.0049</v>
       </c>
       <c r="G43">
         <v>-0.2</v>
       </c>
       <c r="H43">
-        <v>6.07</v>
+        <v>5.5</v>
       </c>
       <c r="I43">
-        <v>8400</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1914,19 +1914,19 @@
         <v>90</v>
       </c>
       <c r="E44">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="F44">
-        <v>0.0067</v>
+        <v>0.0058</v>
       </c>
       <c r="G44">
         <v>-0.19</v>
       </c>
       <c r="H44">
-        <v>7.1</v>
+        <v>6.48</v>
       </c>
       <c r="I44">
-        <v>1400</v>
+        <v>209300</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1943,19 +1943,19 @@
         <v>90</v>
       </c>
       <c r="E45">
-        <v>0.17</v>
+        <v>0.14</v>
       </c>
       <c r="F45">
-        <v>0.0075</v>
+        <v>0.0062</v>
       </c>
       <c r="G45">
         <v>-0.18</v>
       </c>
       <c r="H45">
-        <v>8.24</v>
+        <v>7.57</v>
       </c>
       <c r="I45">
-        <v>24700</v>
+        <v>66600</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1972,19 +1972,19 @@
         <v>90</v>
       </c>
       <c r="E46">
-        <v>0.17</v>
+        <v>0.16</v>
       </c>
       <c r="F46">
-        <v>0.0074</v>
+        <v>0.007</v>
       </c>
       <c r="G46">
         <v>-0.17</v>
       </c>
       <c r="H46">
-        <v>9.5</v>
+        <v>8.789999999999999</v>
       </c>
       <c r="I46">
-        <v>981700</v>
+        <v>554600</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2001,19 +2001,19 @@
         <v>90</v>
       </c>
       <c r="E47">
-        <v>0.2</v>
+        <v>0.14</v>
       </c>
       <c r="F47">
-        <v>0.0086</v>
+        <v>0.006</v>
       </c>
       <c r="G47">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="H47">
-        <v>10.88</v>
+        <v>10.13</v>
       </c>
       <c r="I47">
-        <v>139600</v>
+        <v>57200</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2030,19 +2030,19 @@
         <v>90</v>
       </c>
       <c r="E48">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="F48">
-        <v>0.0089</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="G48">
         <v>-0.16</v>
       </c>
       <c r="H48">
-        <v>12.38</v>
+        <v>11.59</v>
       </c>
       <c r="I48">
-        <v>100600</v>
+        <v>140100</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2059,19 +2059,19 @@
         <v>90</v>
       </c>
       <c r="E49">
-        <v>0.24</v>
+        <v>0.22</v>
       </c>
       <c r="F49">
-        <v>0.0101</v>
+        <v>0.009299999999999999</v>
       </c>
       <c r="G49">
         <v>-0.15</v>
       </c>
       <c r="H49">
-        <v>14</v>
+        <v>13.18</v>
       </c>
       <c r="I49">
-        <v>113900</v>
+        <v>50200</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2088,19 +2088,19 @@
         <v>90</v>
       </c>
       <c r="E50">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="F50">
-        <v>0.0113</v>
+        <v>0.01</v>
       </c>
       <c r="G50">
         <v>-0.14</v>
       </c>
       <c r="H50">
-        <v>15.74</v>
+        <v>14.9</v>
       </c>
       <c r="I50">
-        <v>551500</v>
+        <v>785700</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2117,19 +2117,19 @@
         <v>90</v>
       </c>
       <c r="E51">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="F51">
-        <v>0.0124</v>
+        <v>0.0111</v>
       </c>
       <c r="G51">
         <v>-0.13</v>
       </c>
       <c r="H51">
-        <v>17.6</v>
+        <v>16.74</v>
       </c>
       <c r="I51">
-        <v>220400</v>
+        <v>129900</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2146,19 +2146,19 @@
         <v>90</v>
       </c>
       <c r="E52">
-        <v>0.38</v>
+        <v>0.35</v>
       </c>
       <c r="F52">
-        <v>0.0154</v>
+        <v>0.0141</v>
       </c>
       <c r="G52">
         <v>-0.11</v>
       </c>
       <c r="H52">
-        <v>21.65</v>
+        <v>20.77</v>
       </c>
       <c r="I52">
-        <v>280400</v>
+        <v>55300</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2175,19 +2175,19 @@
         <v>90</v>
       </c>
       <c r="E53">
-        <v>0.42</v>
+        <v>0.41</v>
       </c>
       <c r="F53">
-        <v>0.0168</v>
+        <v>0.0164</v>
       </c>
       <c r="G53">
         <v>-0.1</v>
       </c>
       <c r="H53">
-        <v>23.83</v>
+        <v>22.96</v>
       </c>
       <c r="I53">
-        <v>504600</v>
+        <v>2387300</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2204,19 +2204,19 @@
         <v>90</v>
       </c>
       <c r="E54">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="F54">
-        <v>0.0186</v>
+        <v>0.0174</v>
       </c>
       <c r="G54">
         <v>-0.09</v>
       </c>
       <c r="H54">
-        <v>26.1</v>
+        <v>25.24</v>
       </c>
       <c r="I54">
-        <v>106600</v>
+        <v>112500</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2233,19 +2233,19 @@
         <v>90</v>
       </c>
       <c r="E55">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
       <c r="F55">
-        <v>0.02</v>
+        <v>0.0196</v>
       </c>
       <c r="G55">
         <v>-0.08</v>
       </c>
       <c r="H55">
-        <v>28.45</v>
+        <v>27.61</v>
       </c>
       <c r="I55">
-        <v>131500</v>
+        <v>206800</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2268,7 +2268,7 @@
         <v>-0.08</v>
       </c>
       <c r="H56">
-        <v>28.45</v>
+        <v>27.61</v>
       </c>
       <c r="I56" t="s">
         <v>91</v>
@@ -2288,19 +2288,19 @@
         <v>90</v>
       </c>
       <c r="E57">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F57">
-        <v>0.0225</v>
+        <v>0.0217</v>
       </c>
       <c r="G57">
-        <v>-0.07000000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="H57">
-        <v>30.87</v>
+        <v>30.06</v>
       </c>
       <c r="I57">
-        <v>107100</v>
+        <v>186100</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2317,19 +2317,19 @@
         <v>90</v>
       </c>
       <c r="E58">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="F58">
-        <v>0.025</v>
+        <v>0.0238</v>
       </c>
       <c r="G58">
         <v>-0.07000000000000001</v>
       </c>
       <c r="H58">
-        <v>33.35</v>
+        <v>32.58</v>
       </c>
       <c r="I58">
-        <v>1131200</v>
+        <v>2005900</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2346,19 +2346,19 @@
         <v>90</v>
       </c>
       <c r="E59">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
       <c r="F59">
-        <v>0.0267</v>
+        <v>0.0274</v>
       </c>
       <c r="G59">
         <v>-0.06</v>
       </c>
       <c r="H59">
-        <v>35.89</v>
+        <v>35.15</v>
       </c>
       <c r="I59">
-        <v>66100</v>
+        <v>348500</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2375,19 +2375,19 @@
         <v>90</v>
       </c>
       <c r="E60">
-        <v>0.8100000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="F60">
-        <v>0.0306</v>
+        <v>0.0302</v>
       </c>
       <c r="G60">
         <v>-0.05</v>
       </c>
       <c r="H60">
-        <v>38.46</v>
+        <v>37.77</v>
       </c>
       <c r="I60">
-        <v>130900</v>
+        <v>46500</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2413,10 +2413,10 @@
         <v>-0.04</v>
       </c>
       <c r="H61">
-        <v>41.07</v>
+        <v>40.43</v>
       </c>
       <c r="I61">
-        <v>263400</v>
+        <v>300200</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2432,17 +2432,20 @@
       <c r="D62" t="s">
         <v>90</v>
       </c>
+      <c r="E62">
+        <v>0.95</v>
+      </c>
       <c r="F62">
-        <v>0.037</v>
+        <v>0.0352</v>
       </c>
       <c r="G62">
         <v>-0.03</v>
       </c>
       <c r="H62">
-        <v>43.68</v>
+        <v>43.1</v>
       </c>
       <c r="I62">
-        <v>874900</v>
+        <v>828300</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2459,19 +2462,19 @@
         <v>90</v>
       </c>
       <c r="E63">
-        <v>1.22</v>
+        <v>1.2</v>
       </c>
       <c r="F63">
-        <v>0.0444</v>
+        <v>0.0436</v>
       </c>
       <c r="G63">
         <v>-0.01</v>
       </c>
       <c r="H63">
-        <v>48.91</v>
+        <v>48.45</v>
       </c>
       <c r="I63">
-        <v>465900</v>
+        <v>338200</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2494,7 +2497,7 @@
         <v>-0.01</v>
       </c>
       <c r="H64">
-        <v>48.91</v>
+        <v>48.45</v>
       </c>
       <c r="I64" t="s">
         <v>91</v>
@@ -2514,19 +2517,19 @@
         <v>90</v>
       </c>
       <c r="E65">
-        <v>1.31</v>
+        <v>1.33</v>
       </c>
       <c r="F65">
-        <v>0.0472</v>
+        <v>0.0479</v>
       </c>
       <c r="G65">
         <v>-0</v>
       </c>
       <c r="H65">
-        <v>51.51</v>
+        <v>51.11</v>
       </c>
       <c r="I65">
-        <v>92200</v>
+        <v>122300</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -2543,19 +2546,19 @@
         <v>90</v>
       </c>
       <c r="E66">
-        <v>1.46</v>
+        <v>1.47</v>
       </c>
       <c r="F66">
-        <v>0.0521</v>
+        <v>0.0525</v>
       </c>
       <c r="G66">
         <v>0.01</v>
       </c>
       <c r="H66">
-        <v>54.07</v>
+        <v>53.74</v>
       </c>
       <c r="I66">
-        <v>915500</v>
+        <v>1215600</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -2572,19 +2575,19 @@
         <v>90</v>
       </c>
       <c r="E67">
-        <v>1.69</v>
+        <v>1.74</v>
       </c>
       <c r="F67">
-        <v>0.0593</v>
+        <v>0.0611</v>
       </c>
       <c r="G67">
         <v>0.02</v>
       </c>
       <c r="H67">
-        <v>59.07</v>
+        <v>58.86</v>
       </c>
       <c r="I67">
-        <v>59600</v>
+        <v>84100</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -2607,7 +2610,7 @@
         <v>0.02</v>
       </c>
       <c r="H68">
-        <v>59.07</v>
+        <v>58.86</v>
       </c>
       <c r="I68" t="s">
         <v>91</v>
@@ -2627,19 +2630,19 @@
         <v>90</v>
       </c>
       <c r="E69">
-        <v>1.86</v>
+        <v>1.91</v>
       </c>
       <c r="F69">
-        <v>0.06469999999999999</v>
+        <v>0.0664</v>
       </c>
       <c r="G69">
         <v>0.03</v>
       </c>
       <c r="H69">
-        <v>61.49</v>
+        <v>61.34</v>
       </c>
       <c r="I69">
-        <v>91000</v>
+        <v>39500</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -2656,19 +2659,19 @@
         <v>90</v>
       </c>
       <c r="E70">
-        <v>2</v>
+        <v>2.06</v>
       </c>
       <c r="F70">
-        <v>0.06900000000000001</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="G70">
         <v>0.04</v>
       </c>
       <c r="H70">
-        <v>63.84</v>
+        <v>63.76</v>
       </c>
       <c r="I70">
-        <v>739500</v>
+        <v>582100</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -2685,19 +2688,19 @@
         <v>90</v>
       </c>
       <c r="E71">
-        <v>2.35</v>
+        <v>2.4</v>
       </c>
       <c r="F71">
-        <v>0.07969999999999999</v>
+        <v>0.0814</v>
       </c>
       <c r="G71">
         <v>0.06</v>
       </c>
       <c r="H71">
-        <v>68.33</v>
+        <v>68.36</v>
       </c>
       <c r="I71">
-        <v>7900</v>
+        <v>10700</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -2714,19 +2717,19 @@
         <v>90</v>
       </c>
       <c r="E72">
-        <v>2.76</v>
+        <v>2.82</v>
       </c>
       <c r="F72">
-        <v>0.092</v>
+        <v>0.094</v>
       </c>
       <c r="G72">
         <v>0.08</v>
       </c>
       <c r="H72">
-        <v>72.5</v>
+        <v>72.63</v>
       </c>
       <c r="I72">
-        <v>572700</v>
+        <v>990500</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -2743,19 +2746,19 @@
         <v>90</v>
       </c>
       <c r="E73">
-        <v>3</v>
+        <v>3.21</v>
       </c>
       <c r="F73">
-        <v>0.0984</v>
+        <v>0.1052</v>
       </c>
       <c r="G73">
         <v>0.1</v>
       </c>
       <c r="H73">
-        <v>76.31</v>
+        <v>76.52</v>
       </c>
       <c r="I73">
-        <v>2400</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -2778,7 +2781,7 @@
         <v>0.1</v>
       </c>
       <c r="H74">
-        <v>76.31</v>
+        <v>76.52</v>
       </c>
       <c r="I74" t="s">
         <v>91</v>
@@ -2798,16 +2801,16 @@
         <v>90</v>
       </c>
       <c r="E75">
-        <v>3.02</v>
+        <v>3.36</v>
       </c>
       <c r="F75">
-        <v>0.0982</v>
+        <v>0.1093</v>
       </c>
       <c r="G75">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="H75">
-        <v>78.09</v>
+        <v>78.33</v>
       </c>
       <c r="I75">
         <v>2200</v>
@@ -2827,19 +2830,19 @@
         <v>90</v>
       </c>
       <c r="E76">
-        <v>3.56</v>
+        <v>3.62</v>
       </c>
       <c r="F76">
-        <v>0.1148</v>
+        <v>0.1168</v>
       </c>
       <c r="G76">
         <v>0.11</v>
       </c>
       <c r="H76">
-        <v>79.76000000000001</v>
+        <v>80.03</v>
       </c>
       <c r="I76">
-        <v>13500</v>
+        <v>32200</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -2856,19 +2859,19 @@
         <v>90</v>
       </c>
       <c r="E77">
-        <v>4.05</v>
+        <v>4.07</v>
       </c>
       <c r="F77">
-        <v>0.1286</v>
+        <v>0.1292</v>
       </c>
       <c r="G77">
         <v>0.13</v>
       </c>
       <c r="H77">
-        <v>82.84999999999999</v>
+        <v>83.16</v>
       </c>
       <c r="I77">
-        <v>4000</v>
+        <v>11300</v>
       </c>
     </row>
     <row r="78" spans="1:9">
@@ -2885,19 +2888,19 @@
         <v>90</v>
       </c>
       <c r="E78">
-        <v>3.8</v>
+        <v>4.15</v>
       </c>
       <c r="F78">
-        <v>0.1197</v>
+        <v>0.1307</v>
       </c>
       <c r="G78">
         <v>0.14</v>
       </c>
       <c r="H78">
-        <v>84.25</v>
+        <v>84.58</v>
       </c>
       <c r="I78">
-        <v>5000</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:9">
@@ -2914,19 +2917,19 @@
         <v>90</v>
       </c>
       <c r="E79">
-        <v>4.46</v>
+        <v>4.55</v>
       </c>
       <c r="F79">
-        <v>0.1394</v>
+        <v>0.1422</v>
       </c>
       <c r="G79">
         <v>0.15</v>
       </c>
       <c r="H79">
-        <v>85.56999999999999</v>
+        <v>85.91</v>
       </c>
       <c r="I79">
-        <v>7000</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="80" spans="1:9">
@@ -2949,7 +2952,7 @@
         <v>0.17</v>
       </c>
       <c r="H80">
-        <v>87.95</v>
+        <v>88.31</v>
       </c>
       <c r="I80" t="s">
         <v>91</v>
@@ -2969,19 +2972,19 @@
         <v>90</v>
       </c>
       <c r="E81">
-        <v>6.22</v>
+        <v>5.36</v>
       </c>
       <c r="F81">
-        <v>0.1885</v>
+        <v>0.1624</v>
       </c>
       <c r="G81">
-        <v>0.19</v>
+        <v>0.18</v>
       </c>
       <c r="H81">
-        <v>90.01000000000001</v>
+        <v>90.37</v>
       </c>
       <c r="I81">
-        <v>0</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>